<commit_message>
add: filter by customer email in fetchRedemptions api, isd_code in customer entity
</commit_message>
<xml_diff>
--- a/api/resources/excel/redemption_workbook.xlsx
+++ b/api/resources/excel/redemption_workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>redemption_table</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>customer_email</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
   </si>
 </sst>
 </file>
@@ -499,6 +511,34 @@
         <v>23</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
add: base_order_value in redemptions
</commit_message>
<xml_diff>
--- a/api/resources/excel/redemption_workbook.xlsx
+++ b/api/resources/excel/redemption_workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>redemption_table</t>
   </si>
@@ -67,10 +67,13 @@
     <t>CUSTOMEr5678</t>
   </si>
   <si>
+    <t>base_order_value</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
     <t>discount</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>redeemed_at</t>
@@ -466,7 +469,7 @@
         <v>19</v>
       </c>
       <c r="K5" s="4">
-        <v>100.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="6">
@@ -477,66 +480,80 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="K6" s="4">
+        <v>100.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>27</v>
+      <c r="K9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="2" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>